<commit_message>
add driver fop by xing
</commit_message>
<xml_diff>
--- a/CenterAndCustomerClient/Server-Client protocol.xlsx
+++ b/CenterAndCustomerClient/Server-Client protocol.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LinChiawei\嵌入式作業系統\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m2\Documents\GitHub\eos_pj\CenterAndCustomerClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDEC24E-7B0F-4861-907D-941336A2C182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22875" windowHeight="13605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Command" sheetId="2" r:id="rId2"/>
+    <sheet name="Driver" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -307,24 +309,75 @@
   <si>
     <t>Trigger alarm: broadcast to all client</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>BUZZER</t>
+  </si>
+  <si>
+    <t>BUTTON</t>
+  </si>
+  <si>
+    <t>CAMERA</t>
+  </si>
+  <si>
+    <t>func_trunon</t>
+  </si>
+  <si>
+    <t>func_trunoff</t>
+  </si>
+  <si>
+    <t>lcd_on</t>
+  </si>
+  <si>
+    <t>led_on</t>
+  </si>
+  <si>
+    <t>buz_on</t>
+  </si>
+  <si>
+    <t>btn_on</t>
+  </si>
+  <si>
+    <t>cam_on</t>
+  </si>
+  <si>
+    <t>lcd_off</t>
+  </si>
+  <si>
+    <t>led_off</t>
+  </si>
+  <si>
+    <t>buz_off</t>
+  </si>
+  <si>
+    <t>btn_off</t>
+  </si>
+  <si>
+    <t>cam_off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -371,9 +424,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -384,9 +434,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -394,6 +441,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,89 +727,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="8" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="3" max="4" width="17.6875" customWidth="1"/>
+    <col min="5" max="8" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" s="1"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="2:4">
+      <c r="B3" s="1"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:4">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:4" ht="31.5">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="31.5">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -769,465 +822,466 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="10" width="17.77734375" customWidth="1"/>
+    <col min="2" max="10" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="2:7">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="2:7">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:7" ht="16.25" customHeight="1">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="2:7">
+      <c r="B5" s="8"/>
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="2:7">
+      <c r="B6" s="8"/>
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="5"/>
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="2:7">
+      <c r="B7" s="8"/>
+      <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="2:7">
+      <c r="B8" s="8"/>
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="8" t="s">
+    <row r="9" spans="2:7">
+      <c r="B9" s="8"/>
+      <c r="C9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+    <row r="12" spans="2:7">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="2:7">
+      <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
+    <row r="14" spans="2:7">
+      <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+    <row r="17" spans="2:6">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+    <row r="18" spans="2:6">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="2" t="s">
+    <row r="19" spans="2:6">
+      <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
+    <row r="22" spans="2:6">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="2" t="s">
+    <row r="23" spans="2:6">
+      <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
+    <row r="24" spans="2:6">
+      <c r="C24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
+    <row r="25" spans="2:6">
+      <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="2" t="s">
+    <row r="26" spans="2:6">
+      <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="7"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
+    <row r="27" spans="2:6">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="2" t="s">
+    <row r="30" spans="2:6">
+      <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="2" t="s">
+    <row r="31" spans="2:6">
+      <c r="C31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="2"/>
-      <c r="D34" s="3" t="s">
+    <row r="34" spans="3:10">
+      <c r="C34" s="1"/>
+      <c r="D34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C35" s="2" t="s">
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="3:10">
+      <c r="C35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="2" t="s">
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="3:10">
+      <c r="C36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C37" s="2" t="s">
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" spans="3:10">
+      <c r="C37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="1" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C38" s="2" t="s">
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="3:10">
+      <c r="C38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="1" t="s">
+      <c r="D38" s="2"/>
+      <c r="E38" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C39" s="2" t="s">
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="3:10">
+      <c r="C39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="1" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C42" s="2"/>
-      <c r="D42" s="3" t="s">
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+    </row>
+    <row r="42" spans="3:10">
+      <c r="C42" s="1"/>
+      <c r="D42" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C43" s="2" t="s">
+    <row r="43" spans="3:10">
+      <c r="C43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C44" s="2" t="s">
+    <row r="44" spans="3:10">
+      <c r="C44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C47" s="2"/>
-      <c r="D47" s="1" t="s">
+    <row r="47" spans="3:10">
+      <c r="C47" s="1"/>
+      <c r="D47" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C48" s="2" t="s">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="3:10">
+      <c r="C48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B4:B9"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="E39:G39"/>
@@ -1242,9 +1296,84 @@
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B4:B9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4F06FA-259A-4E90-A082-029D2CD64982}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="6" width="15.5625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add driver fops 2  by xing
</commit_message>
<xml_diff>
--- a/CenterAndCustomerClient/Server-Client protocol.xlsx
+++ b/CenterAndCustomerClient/Server-Client protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m2\Documents\GitHub\eos_pj\CenterAndCustomerClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDEC24E-7B0F-4861-907D-941336A2C182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D07658-EBE9-4104-93C9-0660703D4D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22875" windowHeight="13605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1058" yWindow="300" windowWidth="17010" windowHeight="9780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -326,40 +326,73 @@
     <t>CAMERA</t>
   </si>
   <si>
-    <t>func_trunon</t>
-  </si>
-  <si>
-    <t>func_trunoff</t>
-  </si>
-  <si>
-    <t>lcd_on</t>
-  </si>
-  <si>
-    <t>led_on</t>
-  </si>
-  <si>
-    <t>buz_on</t>
-  </si>
-  <si>
-    <t>btn_on</t>
-  </si>
-  <si>
-    <t>cam_on</t>
-  </si>
-  <si>
-    <t>lcd_off</t>
-  </si>
-  <si>
-    <t>led_off</t>
-  </si>
-  <si>
-    <t>buz_off</t>
-  </si>
-  <si>
-    <t>btn_off</t>
-  </si>
-  <si>
-    <t>cam_off</t>
+    <t>read("lcd",word,strlen(word))</t>
+  </si>
+  <si>
+    <t>write("lcd","",strlen(""))</t>
+  </si>
+  <si>
+    <t>func_trunon(read)</t>
+  </si>
+  <si>
+    <t>func_trunoff(write)</t>
+  </si>
+  <si>
+    <t>func_trunoff(read)</t>
+  </si>
+  <si>
+    <t>func_trunon(write)</t>
+  </si>
+  <si>
+    <t>write("lcd",word,strlen(word))</t>
+  </si>
+  <si>
+    <t>read("lcd","",strlen(""))</t>
+  </si>
+  <si>
+    <t>func/component</t>
+  </si>
+  <si>
+    <t>write("led",1,1)</t>
+  </si>
+  <si>
+    <t>write("led",0,1)</t>
+  </si>
+  <si>
+    <t>write("buz",1,1)</t>
+  </si>
+  <si>
+    <t>write("buz",0,1)</t>
+  </si>
+  <si>
+    <t>write("btn",1,1)</t>
+  </si>
+  <si>
+    <t>write("btn",0,1)</t>
+  </si>
+  <si>
+    <t>write("cam",1,1)</t>
+  </si>
+  <si>
+    <t>write("cam",0,1)</t>
+  </si>
+  <si>
+    <t>read("led","ret_buf","ret_size")</t>
+  </si>
+  <si>
+    <t>read("led","ret_buf","ret_size",)</t>
+  </si>
+  <si>
+    <t>read("buz","ret_buf","ret_size")</t>
+  </si>
+  <si>
+    <t>read("btn","ret_buf","ret_size")</t>
+  </si>
+  <si>
+    <t>read("cam","ret_buf","ret_size")</t>
+  </si>
+  <si>
+    <t>char buf or  word</t>
   </si>
 </sst>
 </file>
@@ -383,12 +416,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -420,7 +459,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -431,22 +470,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,35 +776,35 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -779,34 +812,34 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="31.5">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="31.5">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="1"/>
@@ -871,7 +904,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="16.25" customHeight="1">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -891,7 +924,7 @@
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="8"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -909,7 +942,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="8"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -927,7 +960,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="8"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
@@ -945,7 +978,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="8"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
@@ -963,20 +996,20 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="8"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1029,13 +1062,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="3:6">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="3:6">
       <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1043,7 +1076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="3:6">
       <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1051,7 +1084,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="3:6">
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>50</v>
@@ -1063,7 +1096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="3:6">
       <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="3:6">
       <c r="C24" s="1" t="s">
         <v>31</v>
       </c>
@@ -1091,7 +1124,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="3:6">
       <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1103,7 +1136,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="3:6">
       <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1115,19 +1148,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="5"/>
+    <row r="29" spans="3:6">
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="3:6">
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
@@ -1135,7 +1162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="3:6">
       <c r="C31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1148,16 +1175,16 @@
       <c r="D34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7" t="s">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" spans="3:10">
       <c r="C35" s="1" t="s">
@@ -1166,16 +1193,16 @@
       <c r="D35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7" t="s">
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" spans="3:10">
       <c r="C36" s="1" t="s">
@@ -1184,62 +1211,62 @@
       <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7" t="s">
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37" spans="3:10">
       <c r="C37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7" t="s">
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="3:10">
       <c r="C38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7" t="s">
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="39" spans="3:10">
       <c r="C39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="42" spans="3:10">
       <c r="C42" s="1"/>
@@ -1265,19 +1292,19 @@
     </row>
     <row r="47" spans="3:10">
       <c r="C47" s="1"/>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="3:10">
       <c r="C48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1304,73 +1331,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4F06FA-259A-4E90-A082-029D2CD64982}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="6" width="15.5625" customWidth="1"/>
+    <col min="1" max="1" width="20.4375" customWidth="1"/>
+    <col min="2" max="2" width="26.5625" customWidth="1"/>
+    <col min="3" max="3" width="29.1875" customWidth="1"/>
+    <col min="4" max="4" width="28.4375" customWidth="1"/>
+    <col min="5" max="5" width="29.0625" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="18" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="B5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F3" t="s">
-        <v>86</v>
+      <c r="D5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add driver fops 3 by xing
</commit_message>
<xml_diff>
--- a/CenterAndCustomerClient/Server-Client protocol.xlsx
+++ b/CenterAndCustomerClient/Server-Client protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m2\Documents\GitHub\eos_pj\CenterAndCustomerClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D07658-EBE9-4104-93C9-0660703D4D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C9482A-969D-43D0-A9EB-0C760AEDC406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1058" yWindow="300" windowWidth="17010" windowHeight="9780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,21 +311,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LCD</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>BUZZER</t>
-  </si>
-  <si>
-    <t>BUTTON</t>
-  </si>
-  <si>
-    <t>CAMERA</t>
-  </si>
-  <si>
     <t>read("lcd",word,strlen(word))</t>
   </si>
   <si>
@@ -393,6 +378,21 @@
   </si>
   <si>
     <t>char buf or  word</t>
+  </si>
+  <si>
+    <t>LED(GPIO_21)</t>
+  </si>
+  <si>
+    <t>BUZZER(GPIO_20)</t>
+  </si>
+  <si>
+    <t>BUTTON(GPIO_16)</t>
+  </si>
+  <si>
+    <t>LCD(wiringpi lib)</t>
+  </si>
+  <si>
+    <t>CAMERA (python interface)</t>
   </si>
 </sst>
 </file>
@@ -472,14 +472,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,6 +496,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1529889</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>410340</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>54692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944AE747-2FAB-F48C-1F74-B8E0793DB3CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3087227" y="1223962"/>
+          <a:ext cx="5295538" cy="5145805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -785,10 +834,10 @@
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="1" t="s">
@@ -904,7 +953,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="16.25" customHeight="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -924,7 +973,7 @@
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -942,7 +991,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
@@ -960,7 +1009,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
@@ -978,7 +1027,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
@@ -996,7 +1045,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
@@ -1175,16 +1224,16 @@
       <c r="D34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4" t="s">
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="3:10">
       <c r="C35" s="1" t="s">
@@ -1193,16 +1242,16 @@
       <c r="D35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4" t="s">
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="3:10">
       <c r="C36" s="1" t="s">
@@ -1211,62 +1260,62 @@
       <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" spans="3:10">
       <c r="C37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="38" spans="3:10">
       <c r="C38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" spans="3:10">
       <c r="C39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
     </row>
     <row r="42" spans="3:10">
       <c r="C42" s="1"/>
@@ -1292,19 +1341,19 @@
     </row>
     <row r="47" spans="3:10">
       <c r="C47" s="1"/>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="3:10">
       <c r="C48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1333,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4F06FA-259A-4E90-A082-029D2CD64982}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1348,111 +1397,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="F3" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add lcd wiringpi & new driver api
</commit_message>
<xml_diff>
--- a/CenterAndCustomerClient/Server-Client protocol.xlsx
+++ b/CenterAndCustomerClient/Server-Client protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m2\Documents\GitHub\eos_pj\CenterAndCustomerClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C9482A-969D-43D0-A9EB-0C760AEDC406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A524E5F-E2B4-4350-A9C4-32B80CACAFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1058" yWindow="300" windowWidth="17010" windowHeight="9780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22245" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -311,12 +311,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>read("lcd",word,strlen(word))</t>
-  </si>
-  <si>
-    <t>write("lcd","",strlen(""))</t>
-  </si>
-  <si>
     <t>func_trunon(read)</t>
   </si>
   <si>
@@ -329,57 +323,9 @@
     <t>func_trunon(write)</t>
   </si>
   <si>
-    <t>write("lcd",word,strlen(word))</t>
-  </si>
-  <si>
-    <t>read("lcd","",strlen(""))</t>
-  </si>
-  <si>
     <t>func/component</t>
   </si>
   <si>
-    <t>write("led",1,1)</t>
-  </si>
-  <si>
-    <t>write("led",0,1)</t>
-  </si>
-  <si>
-    <t>write("buz",1,1)</t>
-  </si>
-  <si>
-    <t>write("buz",0,1)</t>
-  </si>
-  <si>
-    <t>write("btn",1,1)</t>
-  </si>
-  <si>
-    <t>write("btn",0,1)</t>
-  </si>
-  <si>
-    <t>write("cam",1,1)</t>
-  </si>
-  <si>
-    <t>write("cam",0,1)</t>
-  </si>
-  <si>
-    <t>read("led","ret_buf","ret_size")</t>
-  </si>
-  <si>
-    <t>read("led","ret_buf","ret_size",)</t>
-  </si>
-  <si>
-    <t>read("buz","ret_buf","ret_size")</t>
-  </si>
-  <si>
-    <t>read("btn","ret_buf","ret_size")</t>
-  </si>
-  <si>
-    <t>read("cam","ret_buf","ret_size")</t>
-  </si>
-  <si>
-    <t>char buf or  word</t>
-  </si>
-  <si>
     <t>LED(GPIO_21)</t>
   </si>
   <si>
@@ -393,6 +339,46 @@
   </si>
   <si>
     <t>CAMERA (python interface)</t>
+  </si>
+  <si>
+    <t>write(file,"led_1",strlen(1))</t>
+  </si>
+  <si>
+    <t>write(file,"led_0",strlen(0))</t>
+  </si>
+  <si>
+    <t>func_open</t>
+  </si>
+  <si>
+    <t>open("/dev/eos7_driver", O_RDWR)</t>
+  </si>
+  <si>
+    <t>write(file,"lcd_word",strlen(word))</t>
+  </si>
+  <si>
+    <t>write(file,"lcd_0",strlen("0"))</t>
+  </si>
+  <si>
+    <t>write(file,"buz_1",strlen(1))</t>
+  </si>
+  <si>
+    <t>write(file,"buz_0",strlen(0))</t>
+  </si>
+  <si>
+    <t>write(file,"btn_1",strlen(1))</t>
+  </si>
+  <si>
+    <t>write(file,"btn_0",strlen(0))</t>
+  </si>
+  <si>
+    <t>write(file,"cam_1",strlen(1))</t>
+  </si>
+  <si>
+    <t>write(file,"cam_0",strlen(1))</t>
+  </si>
+  <si>
+    <t>read(file,"btn",0)
+read(file,"btn_ret_buf",strlen(ret_size))</t>
   </si>
 </sst>
 </file>
@@ -430,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -453,13 +439,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -480,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,16 +502,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1529889</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>144002</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>410340</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2520128</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>54692</xdr:rowOff>
+      <xdr:rowOff>164230</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -534,7 +534,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3087227" y="1223962"/>
+          <a:off x="4596940" y="1333500"/>
           <a:ext cx="5295538" cy="5145805"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1380,125 +1380,112 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4F06FA-259A-4E90-A082-029D2CD64982}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20.4375" customWidth="1"/>
-    <col min="2" max="2" width="26.5625" customWidth="1"/>
-    <col min="3" max="3" width="29.1875" customWidth="1"/>
-    <col min="4" max="4" width="28.4375" customWidth="1"/>
-    <col min="5" max="5" width="29.0625" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="38.3125" customWidth="1"/>
+    <col min="4" max="4" width="38.1875" customWidth="1"/>
+    <col min="5" max="5" width="38.125" customWidth="1"/>
     <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="37.15" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="40.5" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>89</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>92</v>
+      <c r="B6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>